<commit_message>
updated the tab name
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_SYSTEMCONSTRAINTS.xlsx
+++ b/LH_TESTCASES/LH_TC_SYSTEMCONSTRAINTS.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce4e295319cf0be1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gehad\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5EB3D8E-C389-4747-A0AC-47C025D481C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F5EB3D8E-C389-4747-A0AC-47C025D481C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{643F10FD-C51D-464A-BED9-DAD756E95A41}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LOGIN-TC-SHEET" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCases-SHEET" sheetId="1" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -364,203 +364,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -660,6 +463,203 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -674,33 +674,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:K8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="TC_ID" dataDxfId="2"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SRS_ID" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Title" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Preconditions" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Test Data" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Steps" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Expected Results" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Provided By" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Priority" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Severity" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="TC_ID" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="SRS_ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Title" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Preconditions" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Test Data" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Steps" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Expected Results" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Provided By" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Priority" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Severity" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:D4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table3" displayName="Table3" ref="A1:D4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5">
   <autoFilter ref="A1:D4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Version number" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Updated section" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Version number" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Updated section" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -971,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="44" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="44" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1272,7 +1272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+    <sheetView zoomScale="118" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adjustments according new SRSs
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_SYSTEMCONSTRAINTS.xlsx
+++ b/LH_TESTCASES/LH_TC_SYSTEMCONSTRAINTS.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ce4e295319cf0be1/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\TCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A95B5BF-897F-441A-92EA-D1155D9693D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_SYSTEMCONSTRAINTS" sheetId="1" r:id="rId1"/>
     <sheet name="VESRION HISTORY" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LH_TC_SYSTEMCONSTRAINTS!$A$8:$I$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LH_TC_SYSTEMCONSTRAINTS!$A$8:$I$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
   <si>
     <t>Preconditions</t>
   </si>
@@ -89,9 +88,6 @@
     <t>priority</t>
   </si>
   <si>
-    <t>SRS-SYS-001</t>
-  </si>
-  <si>
     <t>Gehad Ashry</t>
   </si>
   <si>
@@ -101,86 +97,22 @@
     <t>System Constraints</t>
   </si>
   <si>
-    <t>Validate that the web application can be deployed to a desktop environment and functions correctly without runtime or network errors.</t>
-  </si>
-  <si>
-    <t>1-Web application is built and packaged.
-2-Chrome version 135.0.7049.96 is installed on Windows 10.</t>
-  </si>
-  <si>
-    <t>Application build files (HTML, CSS, JS, etc.)</t>
-  </si>
-  <si>
-    <t>1-Deploy the application to a test server.
-2-Open the application URL in Chrome (Windows 10).
-3-Open Developer Tools (F12).
-4-Inspect the Console for JavaScript errors.
-5-Inspect the Network tab for any failed requests (4xx/5xx).</t>
-  </si>
-  <si>
-    <t>1-Application interface loads without issues.
-2-No JavaScript/runtime errors are shown in Console.
-3-No failed network requests appear (all requests return 2xx/3xx).</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>High</t>
   </si>
   <si>
-    <t>Ensure the application runs properly and error-free on commonly used desktop browsers (latest stable versions).</t>
-  </si>
-  <si>
     <t>Application is deployed on a test server.</t>
   </si>
   <si>
-    <t>1-Firefox v137
-2-Edge v135</t>
-  </si>
-  <si>
-    <t>1-Open the application on each supported browser.
-2-Navigate through the homepage and all core pages.
-3-Open DevTools (F12) on each browser.
-4-Check Console for errors.
-5-Check Network tab for failed requests.</t>
-  </si>
-  <si>
-    <t>1-Pages render without distortion in both browsers.
-2-Buttons, links, and forms are fully functional.
-3-No JavaScript errors or failed network requests observed.</t>
-  </si>
-  <si>
     <t>LH-TC-SYSTEMCONSTRAINTS-001</t>
   </si>
   <si>
     <t>LH-TC-SYSTEMCONSTRAINTS-002</t>
   </si>
   <si>
-    <t>LH-TC-SYSTEMCONSTRAINTS-003</t>
-  </si>
-  <si>
-    <t>LH-TC-SYSTEMCONSTRAINTS-004</t>
-  </si>
-  <si>
-    <t>Verify that the application layout and user interface elements remain fully functional and accessible when viewed at the minimum supported desktop resolution of 1024x768 pixels.</t>
-  </si>
-  <si>
-    <t>Screen resolution: 1024x768</t>
-  </si>
-  <si>
-    <t>1-Set the screen resolution to 1024x768 or resize the browser window to this size.
-2-Open the application homepage.
-3-Navigate through all main pages.
-4-Observe the layout, alignment, and visibility of elements.
-5-Attempt to interact with all navigation elements, buttons, forms, and content sections.</t>
-  </si>
-  <si>
     <t>Medium</t>
-  </si>
-  <si>
-    <t>1-No horizontal scrolling needed.
-2-Navigation, text, and inputs are fully accessible.</t>
   </si>
   <si>
     <t>Ensure the application's user interface adjusts correctly and remains visually consistent across a range of widely used desktop screen resolutions.</t>
@@ -215,11 +147,122 @@
   <si>
     <t>v1.1</t>
   </si>
+  <si>
+    <t>Ahmed Abuzaid</t>
+  </si>
+  <si>
+    <t>LH-SRS-SYS-001</t>
+  </si>
+  <si>
+    <t>Ensure the application runs properly and error-free on commonly used desktop browsers</t>
+  </si>
+  <si>
+    <t>1-Pages render without distortion in any browser.
+2-Buttons, links, and forms are fully functional.
+3-No JavaScript errors or failed network requests observed.</t>
+  </si>
+  <si>
+    <t>1-Open the application on each supported browser.
+2-Navigate through the homepage and all core pages.
+3-Open DevTools (F12) on each browser.
+4-Check Console for errors.</t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>chrom browser
+firfox browser</t>
+  </si>
+  <si>
+    <t>Verifying that each user receives a unique ID upon registration</t>
+  </si>
+  <si>
+    <t>1. The system is operational.
+2. The user registration form is accessible.</t>
+  </si>
+  <si>
+    <t>1-first user:
+Email: user1@domain.com
+Username: user111
+Password: Pass@1234
+2-second user:
+Email: user2@domain.com
+Username: user222
+Password: Pass@1234</t>
+  </si>
+  <si>
+    <t>1- Each user receives a unique user ID.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensuring generated user IDs follow the required format UXXX.  </t>
+  </si>
+  <si>
+    <t>1. The system is operational.  
+2. The user registration form is accessible.</t>
+  </si>
+  <si>
+    <t>1-Email: user3@domain.com
+2-Username: user333
+3-Password: Pass@1234</t>
+  </si>
+  <si>
+    <t>1- The user ID generated is in the format UXXX (e.g., U001).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Checking that user IDs are generated sequentially.</t>
+  </si>
+  <si>
+    <t>1-first user:
+Email: user4@domain.com
+Username: user444
+Password: Pass@1234
+2-second user:
+Email: user5@domain.com
+Username: user555
+Password: Pass@1234</t>
+  </si>
+  <si>
+    <t>1- The second user ID is the next sequential ID after the first user ID (e.g., if the first user ID is U001, the second is U002).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LH-SRS-SYS-002
+</t>
+  </si>
+  <si>
+    <t>LH-TC-SYSTEMCONSTRAINTS-003</t>
+  </si>
+  <si>
+    <t>LH-TC-SYSTEMCONSTRAINTS-004</t>
+  </si>
+  <si>
+    <t>LH-TC-SYSTEMCONSTRAINTS-005</t>
+  </si>
+  <si>
+    <t>1- Navigate to the sign up page on the browser
+2- Enter valid email.
+3- Enter valid username.
+4- Enter valid password.
+5- Click Register.
+5- check the user ID in database
+7- Register another new user with a different valid email, username, and password and then check the user ID in database</t>
+  </si>
+  <si>
+    <t>1- Navigate to the sign up page on the browser
+2- Enter valid email.
+3- Enter valid username.
+4- Enter valid password.
+5- Click Register.
+6-check the user ID in database</t>
+  </si>
+  <si>
+    <t>Adjustemnts according new SRSs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -380,11 +423,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -404,20 +460,49 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -436,29 +521,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,23 +638,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -626,23 +673,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -818,14 +848,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="C11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" style="5" customWidth="1"/>
     <col min="2" max="2" width="43.140625" style="1" customWidth="1"/>
@@ -835,7 +865,7 @@
     <col min="6" max="6" width="54.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="108.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="16"/>
+    <col min="9" max="9" width="25.7109375" style="14"/>
     <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="21.140625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
@@ -845,44 +875,44 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
+      <c r="B2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="15"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
+      <c r="B4" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -913,7 +943,7 @@
       <c r="F8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -926,138 +956,162 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="14" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="23" t="s">
+    <row r="9" spans="1:10" ht="84" x14ac:dyDescent="0.35">
+      <c r="A9" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="26" t="s">
+    </row>
+    <row r="10" spans="1:10" ht="189" x14ac:dyDescent="0.35">
+      <c r="A10" s="32"/>
+      <c r="B10" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="23" t="s">
+      <c r="C10" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="105" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="147" x14ac:dyDescent="0.35">
-      <c r="A11" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="23" t="s">
+    </row>
+    <row r="11" spans="1:10" ht="168" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="189" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="30" t="s">
+      <c r="E11" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="G11" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="H11" s="17"/>
+      <c r="I11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="126" x14ac:dyDescent="0.35">
+      <c r="A12" s="25"/>
+      <c r="B12" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="23" t="s">
+      <c r="E12" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E13" s="25"/>
+      <c r="G12" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="168" x14ac:dyDescent="0.35">
+      <c r="A13" s="25"/>
+      <c r="B13" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E14" s="25"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E15" s="25"/>
+      <c r="I14" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A8:I9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <mergeCells count="4">
+  <autoFilter ref="A8:I8"/>
+  <mergeCells count="6">
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
@@ -1068,7 +1122,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1048576">
       <formula1>"Pass, Fail, Blocked, N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1077,86 +1131,94 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>45766</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="13">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="12">
         <v>45769</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:4" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:4" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="12">
+        <v>45966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" s="9" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>